<commit_message>
add link to task 6.1 to lab14
</commit_message>
<xml_diff>
--- a/src/code-complete-status.xlsx
+++ b/src/code-complete-status.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="9240" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>главы</t>
   </si>
@@ -124,13 +124,16 @@
   </si>
   <si>
     <t>12.3</t>
+  </si>
+  <si>
+    <t>9.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,17 +171,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -216,7 +224,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -250,6 +258,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -284,9 +293,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -459,19 +469,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -487,7 +497,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,7 +541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -543,28 +553,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B35" si="0">SUM(C4:N4)</f>
+        <f t="shared" ref="B4:B36" si="0">SUM(C4:N4)</f>
         <v>1</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -573,7 +586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -582,7 +595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -591,7 +604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -600,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -612,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -621,7 +634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -630,7 +643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -639,221 +652,233 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="1" t="s">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="1" t="s">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1" t="s">
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1" t="s">
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1" t="s">
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1" t="s">
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1" t="s">
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1" t="s">
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1" t="s">
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="1" t="s">
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -868,12 +893,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -881,12 +906,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>

<commit_message>
add links to parts of chapter 7 of code-complete to lab 12
</commit_message>
<xml_diff>
--- a/src/code-complete-status.xlsx
+++ b/src/code-complete-status.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="9240" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>главы</t>
   </si>
@@ -127,13 +127,19 @@
   </si>
   <si>
     <t>9.2</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>прогресс:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,9 +177,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -184,9 +203,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -224,7 +243,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -258,7 +277,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -293,10 +311,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -469,22 +486,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
+    <row r="1" spans="1:15">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -495,410 +510,442 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1">
+        <f>SUM(N3:N1000)/COUNT(N3:N1000)</f>
+        <v>0.45714285714285713</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>9</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
+      <c r="K2">
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <v>14</v>
+      </c>
+      <c r="M2">
+        <v>15</v>
+      </c>
+      <c r="N2" t="s">
         <v>28</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="G2">
-        <v>7</v>
-      </c>
-      <c r="H2">
-        <v>8</v>
-      </c>
-      <c r="I2">
-        <v>9</v>
-      </c>
-      <c r="J2">
-        <v>10</v>
-      </c>
-      <c r="K2">
-        <v>12</v>
-      </c>
-      <c r="L2">
-        <v>13</v>
-      </c>
-      <c r="M2">
-        <v>14</v>
-      </c>
-      <c r="N2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <f>SUM(C3:N3)</f>
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N37" si="0">SUM(B3:M3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <f t="shared" ref="B4:B36" si="0">SUM(C4:N4)</f>
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="N29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="N31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="N33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="N34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B34">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="N36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B36">
+      <c r="N37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="B1:M1"/>
   </mergeCells>
+  <conditionalFormatting sqref="N3:N37">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -906,12 +953,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>

<commit_message>
add chapter 8.4 and 7.5 to lab 13 and 12 respectively
</commit_message>
<xml_diff>
--- a/src/code-complete-status.xlsx
+++ b/src/code-complete-status.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>главы</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>8.4</t>
-  </si>
-  <si>
-    <t>8.6</t>
   </si>
   <si>
     <t>10.2</t>
@@ -487,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -511,11 +508,11 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O1">
-        <f>SUM(N3:N1000)/COUNT(N3:N1000)</f>
-        <v>0.45714285714285713</v>
+        <f>SUM(N3:N999)/COUNT(N3:N999)</f>
+        <v>0.52941176470588236</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -559,7 +556,7 @@
         <v>15</v>
       </c>
       <c r="N2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -570,7 +567,7 @@
         <v>1</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N37" si="0">SUM(B3:M3)</f>
+        <f t="shared" ref="N3:N36" si="0">SUM(B3:M3)</f>
         <v>1</v>
       </c>
     </row>
@@ -600,7 +597,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -650,9 +647,12 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
       <c r="N10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -680,25 +680,31 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>35</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15">
+        <v>12</v>
+      </c>
+      <c r="B15">
         <v>1</v>
       </c>
       <c r="N15">
@@ -708,19 +714,16 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="N16">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="N17">
         <f t="shared" si="0"/>
@@ -729,16 +732,19 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
       </c>
       <c r="N18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -750,7 +756,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -786,14 +792,11 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N23">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -888,23 +891,23 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
       </c>
       <c r="N34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="N35">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -912,15 +915,6 @@
         <v>26</v>
       </c>
       <c r="N36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -929,7 +923,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:M1"/>
   </mergeCells>
-  <conditionalFormatting sqref="N3:N37">
+  <conditionalFormatting sqref="N3:N36">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add links to chapters 10.8 and 11.2 to lab06
</commit_message>
<xml_diff>
--- a/src/code-complete-status.xlsx
+++ b/src/code-complete-status.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>главы</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>11.1</t>
-  </si>
-  <si>
-    <t>10.3</t>
   </si>
   <si>
     <t>11.2</t>
@@ -484,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -508,11 +505,11 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O1">
-        <f>SUM(N3:N999)/COUNT(N3:N999)</f>
-        <v>0.52941176470588236</v>
+        <f>SUM(N3:N998)/COUNT(N3:N998)</f>
+        <v>0.5757575757575758</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -567,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N36" si="0">SUM(B3:M3)</f>
+        <f>IF(SUM(B3:M3)&gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -579,7 +576,7 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="N4:N35" si="0">IF(SUM(B4:M4)&gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -597,7 +594,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -690,7 +687,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -714,27 +711,36 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
       </c>
       <c r="N16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
       </c>
       <c r="N17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="E18">
         <v>1</v>
       </c>
       <c r="N18">
@@ -744,7 +750,7 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -780,19 +786,16 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N22">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N23">
         <f t="shared" si="0"/>
@@ -801,7 +804,7 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N24">
         <f t="shared" si="0"/>
@@ -810,7 +813,7 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N25">
         <f t="shared" si="0"/>
@@ -819,7 +822,7 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N26">
         <f t="shared" si="0"/>
@@ -828,7 +831,7 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N27">
         <f t="shared" si="0"/>
@@ -837,7 +840,7 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N28">
         <f t="shared" si="0"/>
@@ -846,7 +849,7 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N29">
         <f t="shared" si="0"/>
@@ -855,7 +858,7 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N30">
         <f t="shared" si="0"/>
@@ -864,7 +867,7 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N31">
         <f t="shared" si="0"/>
@@ -873,7 +876,7 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N32">
         <f t="shared" si="0"/>
@@ -882,39 +885,30 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
       </c>
       <c r="N33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="N34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -923,7 +917,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:M1"/>
   </mergeCells>
-  <conditionalFormatting sqref="N3:N36">
+  <conditionalFormatting sqref="N3:N35">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add link to chapter 8.3 to lab 09 fix some typos
</commit_message>
<xml_diff>
--- a/src/code-complete-status.xlsx
+++ b/src/code-complete-status.xlsx
@@ -484,7 +484,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -509,7 +509,7 @@
       </c>
       <c r="O1">
         <f>SUM(N3:N998)/COUNT(N3:N998)</f>
-        <v>0.5757575757575758</v>
+        <v>0.60606060606060608</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -668,9 +668,12 @@
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
       <c r="N12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:15">

</xml_diff>

<commit_message>
add links to chapter 15.1 and 15.2 to lab05
</commit_message>
<xml_diff>
--- a/src/code-complete-status.xlsx
+++ b/src/code-complete-status.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>главы</t>
   </si>
@@ -60,12 +60,6 @@
     <t>10.8</t>
   </si>
   <si>
-    <t>14.1</t>
-  </si>
-  <si>
-    <t>14.2</t>
-  </si>
-  <si>
     <t>15.1</t>
   </si>
   <si>
@@ -127,6 +121,9 @@
   </si>
   <si>
     <t>прогресс:</t>
+  </si>
+  <si>
+    <t>19.4</t>
   </si>
 </sst>
 </file>
@@ -173,7 +170,19 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -481,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -505,11 +514,11 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O1">
-        <f>SUM(N3:N998)/COUNT(N3:N998)</f>
-        <v>0.60606060606060608</v>
+        <f>SUM(N3:N997)/COUNT(N3:N997)</f>
+        <v>0.6875</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -553,7 +562,7 @@
         <v>15</v>
       </c>
       <c r="N2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -576,7 +585,7 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N35" si="0">IF(SUM(B4:M4)&gt;0,1,0)</f>
+        <f t="shared" ref="N4:N34" si="0">IF(SUM(B4:M4)&gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -594,7 +603,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -690,7 +699,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -726,7 +735,7 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -738,7 +747,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -753,7 +762,7 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -765,7 +774,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -777,7 +786,7 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -791,18 +800,24 @@
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
       <c r="N22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
       <c r="N23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -834,7 +849,7 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="N27">
         <f t="shared" si="0"/>
@@ -843,7 +858,7 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N28">
         <f t="shared" si="0"/>
@@ -852,7 +867,7 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N29">
         <f t="shared" si="0"/>
@@ -861,7 +876,7 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N30">
         <f t="shared" si="0"/>
@@ -870,7 +885,7 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N31">
         <f t="shared" si="0"/>
@@ -879,39 +894,30 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
       </c>
       <c r="N32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="N33">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
-      <c r="A35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -920,8 +926,8 @@
   <mergeCells count="1">
     <mergeCell ref="B1:M1"/>
   </mergeCells>
-  <conditionalFormatting sqref="N3:N35">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="N3:N34">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
remove links from nav sidebar add links to multiple chapters from code-complete
</commit_message>
<xml_diff>
--- a/src/code-complete-status.xlsx
+++ b/src/code-complete-status.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>главы</t>
   </si>
@@ -124,6 +124,15 @@
   </si>
   <si>
     <t>19.4</t>
+  </si>
+  <si>
+    <t>12.8</t>
+  </si>
+  <si>
+    <t>16.1</t>
+  </si>
+  <si>
+    <t>19.3</t>
   </si>
 </sst>
 </file>
@@ -490,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -517,8 +526,8 @@
         <v>34</v>
       </c>
       <c r="O1">
-        <f>SUM(N3:N997)/COUNT(N3:N997)</f>
-        <v>0.6875</v>
+        <f>SUM(N3:N1000)/COUNT(N3:N1000)</f>
+        <v>0.78787878787878785</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -585,7 +594,7 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N34" si="0">IF(SUM(B4:M4)&gt;0,1,0)</f>
+        <f t="shared" ref="N4:N37" si="0">IF(SUM(B4:M4)&gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -798,9 +807,9 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22">
+        <v>36</v>
+      </c>
+      <c r="G22">
         <v>1</v>
       </c>
       <c r="N22">
@@ -810,7 +819,7 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -822,61 +831,71 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="N24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
       </c>
       <c r="N26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
       </c>
       <c r="N27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
       </c>
       <c r="N28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N29">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="N30">
         <f t="shared" si="0"/>
@@ -885,7 +904,7 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="N31">
         <f t="shared" si="0"/>
@@ -894,19 +913,16 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="N32">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N33">
         <f t="shared" si="0"/>
@@ -915,9 +931,39 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N34">
+      <c r="N37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -926,8 +972,8 @@
   <mergeCells count="1">
     <mergeCell ref="B1:M1"/>
   </mergeCells>
-  <conditionalFormatting sqref="N3:N34">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="N3:N37">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add links to chapters 23.1-23.3 to lab 06 add link to chapter 19.4 to lab 05
</commit_message>
<xml_diff>
--- a/src/code-complete-status.xlsx
+++ b/src/code-complete-status.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="9240" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>главы</t>
   </si>
@@ -133,13 +133,16 @@
   </si>
   <si>
     <t>19.3</t>
+  </si>
+  <si>
+    <t>23.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,9 +180,33 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -215,9 +242,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -255,7 +282,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -289,6 +316,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -323,9 +351,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -498,16 +527,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -526,11 +555,11 @@
         <v>34</v>
       </c>
       <c r="O1">
-        <f>SUM(N3:N1000)/COUNT(N3:N1000)</f>
-        <v>0.78787878787878785</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+        <f>SUM(N3:N1001)/COUNT(N3:N1001)</f>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +603,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -586,7 +615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -594,11 +623,11 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N37" si="0">IF(SUM(B4:M4)&gt;0,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <f t="shared" ref="N4:N38" si="0">IF(SUM(B4:M4)&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -610,7 +639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -622,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -634,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -646,7 +675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -658,7 +687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -670,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -682,7 +711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -694,7 +723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -706,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -718,7 +747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -730,7 +759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -742,7 +771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -754,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -769,7 +798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -781,7 +810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -793,7 +822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -805,7 +834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -817,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -829,7 +858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -841,15 +870,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -861,7 +894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
@@ -873,7 +906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
@@ -885,85 +918,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="N29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
       <c r="N30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
       <c r="N31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
       <c r="N32">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
-      <c r="A33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N33">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
-      <c r="A34" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N34">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
-      <c r="A35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="N35">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N37">
+      <c r="N38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -972,8 +1030,8 @@
   <mergeCells count="1">
     <mergeCell ref="B1:M1"/>
   </mergeCells>
-  <conditionalFormatting sqref="N3:N37">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="N3:N38">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -983,12 +1041,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -996,12 +1054,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>

<commit_message>
add links to chapters 34.1, 31.1, 30.2 to labs 14, 06, 01 respectively
</commit_message>
<xml_diff>
--- a/src/code-complete-status.xlsx
+++ b/src/code-complete-status.xlsx
@@ -84,15 +84,9 @@
     <t>30</t>
   </si>
   <si>
-    <t>31.1</t>
-  </si>
-  <si>
     <t>33</t>
   </si>
   <si>
-    <t>34</t>
-  </si>
-  <si>
     <t>использована?</t>
   </si>
   <si>
@@ -136,6 +130,12 @@
   </si>
   <si>
     <t>23.3</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>34.1</t>
   </si>
 </sst>
 </file>
@@ -182,43 +182,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <condense val="0"/>
@@ -531,7 +495,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,11 +516,11 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O1">
         <f>SUM(N3:N1001)/COUNT(N3:N1001)</f>
-        <v>0.88888888888888884</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -600,7 +564,7 @@
         <v>15</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -641,7 +605,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -737,7 +701,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -773,7 +737,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -785,7 +749,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -800,7 +764,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -812,7 +776,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -824,7 +788,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -836,7 +800,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -872,7 +836,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -920,7 +884,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -932,7 +896,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -968,7 +932,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -982,23 +946,29 @@
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
       <c r="N34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
       </c>
       <c r="N35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1010,20 +980,26 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
       </c>
       <c r="N37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
       </c>
       <c r="N38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1031,7 +1007,7 @@
     <mergeCell ref="B1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="N3:N38">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>